<commit_message>
data finished and worked on graph
</commit_message>
<xml_diff>
--- a/Data/End of Day/End of Day_23_Graph.xlsx
+++ b/Data/End of Day/End of Day_23_Graph.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oliviarandell/Documents/GitHub/GGEESummer23/Data/End of Day/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D18986E-05AB-FE4A-A3E6-5C70D653B901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC12E29-3B5F-8541-B02C-C4D7C371FA0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12260" yWindow="500" windowWidth="15360" windowHeight="15940" firstSheet="4" activeTab="8" xr2:uid="{577BAB1A-2EED-D742-95AC-6D0DE0AFCAEE}"/>
+    <workbookView xWindow="14520" yWindow="500" windowWidth="14280" windowHeight="15940" firstSheet="6" activeTab="10" xr2:uid="{577BAB1A-2EED-D742-95AC-6D0DE0AFCAEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Feeling" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,9 @@
     <sheet name="enjoy_do" sheetId="4" r:id="rId6"/>
     <sheet name="TEST" sheetId="7" r:id="rId7"/>
     <sheet name="Feeling Stacked" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet4" sheetId="11" r:id="rId9"/>
-    <sheet name="Identity Stacked" sheetId="9" r:id="rId10"/>
-    <sheet name="Find Stacked " sheetId="10" r:id="rId11"/>
+    <sheet name="Identity Stacked" sheetId="9" r:id="rId9"/>
+    <sheet name="Find Stacked " sheetId="10" r:id="rId10"/>
+    <sheet name="Enjoy Stacked" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="37">
   <si>
     <t>Question</t>
   </si>
@@ -262,10 +262,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -842,18 +840,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ABF019-0EA5-9346-A662-004F30A49F1A}">
-  <dimension ref="A1:E46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18683B-ECE9-E342-B333-4B4395343288}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42:C46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -875,767 +873,512 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2">
-        <v>74</v>
-      </c>
-      <c r="E2" s="2">
-        <v>26.90909090909091</v>
+        <v>14</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>2.9090909090909092</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="2">
-        <v>84</v>
-      </c>
-      <c r="E3" s="2">
-        <v>30.545454545454547</v>
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <v>2.9090909090909092</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="2">
-        <v>70</v>
-      </c>
-      <c r="E4" s="2">
-        <v>25.454545454545453</v>
+      <c r="D4">
+        <v>29</v>
+      </c>
+      <c r="E4">
+        <v>10.545454545454545</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="2">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8.3636363636363633</v>
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
+        <v>20.363636363636363</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="2">
-        <v>24</v>
-      </c>
-      <c r="E6" s="2">
-        <v>8.7272727272727284</v>
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>174</v>
+      </c>
+      <c r="E6">
+        <v>63.272727272727266</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2">
-        <v>94</v>
-      </c>
-      <c r="E7" s="2">
-        <v>37.6</v>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="2">
-        <v>56</v>
-      </c>
-      <c r="E8" s="2">
-        <v>22.400000000000002</v>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1.6666666666666667</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="2">
-        <v>61</v>
-      </c>
-      <c r="E9" s="2">
-        <v>24.4</v>
+      <c r="D9" s="11">
+        <v>17</v>
+      </c>
+      <c r="E9" s="11">
+        <v>7.0833333300000003</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="2">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2">
-        <v>6.8000000000000007</v>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>65</v>
+      </c>
+      <c r="E10">
+        <v>27.083333333333332</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="2">
-        <v>22</v>
-      </c>
-      <c r="E11" s="2">
-        <v>8.7999999999999989</v>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>150</v>
+      </c>
+      <c r="E11">
+        <v>62.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="2">
-        <v>154</v>
-      </c>
-      <c r="E12" s="2">
-        <v>42.777777777777779</v>
+        <v>14</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>2.5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="2">
-        <v>67</v>
-      </c>
-      <c r="E13" s="2">
-        <v>18.611111111111111</v>
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>5.5555555555555554</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="2">
-        <v>77</v>
-      </c>
-      <c r="E14" s="2">
-        <v>21.388888888888889</v>
+      <c r="D14">
+        <v>44</v>
+      </c>
+      <c r="E14">
+        <v>12.222222222222221</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="2">
-        <v>22</v>
-      </c>
-      <c r="E15" s="2">
-        <v>6.1111111111111107</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>68</v>
+      </c>
+      <c r="E15">
+        <v>18.888888888888889</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="2">
-        <v>40</v>
-      </c>
-      <c r="E16" s="2">
-        <v>11.111111111111111</v>
+        <v>14</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>219</v>
+      </c>
+      <c r="E16">
+        <v>60.833333333333329</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="2">
-        <v>76</v>
-      </c>
-      <c r="E17" s="2">
-        <v>27.636363636363637</v>
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17">
+        <v>63</v>
+      </c>
+      <c r="E17">
+        <v>22.90909090909091</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="2">
-        <v>95</v>
-      </c>
-      <c r="E18" s="2">
-        <v>34.545454545454547</v>
+        <v>9</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <v>21.818181818181817</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="2">
-        <v>64</v>
-      </c>
-      <c r="E19" s="2">
-        <v>23.272727272727273</v>
+      <c r="D19">
+        <v>67</v>
+      </c>
+      <c r="E19">
+        <v>24.363636363636363</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="2">
-        <v>25</v>
-      </c>
-      <c r="E20" s="2">
-        <v>9.0909090909090917</v>
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>58</v>
+      </c>
+      <c r="E20">
+        <v>21.09090909090909</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="2">
-        <v>15</v>
-      </c>
-      <c r="E21" s="2">
-        <v>5.4545454545454541</v>
+        <v>9</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>27</v>
+      </c>
+      <c r="E21">
+        <v>9.8181818181818183</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="2">
-        <v>81</v>
-      </c>
-      <c r="E22" s="2">
-        <v>32.4</v>
+      <c r="C22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>55</v>
+      </c>
+      <c r="E22">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="2">
-        <v>79</v>
-      </c>
-      <c r="E23" s="2">
-        <v>31.6</v>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23">
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D24" s="2">
-        <v>66</v>
-      </c>
-      <c r="E24" s="2">
-        <v>26.400000000000002</v>
+      <c r="D24">
+        <v>62</v>
+      </c>
+      <c r="E24">
+        <v>24.8</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="2">
-        <v>13</v>
-      </c>
-      <c r="E25" s="2">
-        <v>5.2</v>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>57</v>
+      </c>
+      <c r="E25">
+        <v>22.8</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26">
         <v>36</v>
       </c>
-      <c r="D26" s="2">
-        <v>11</v>
-      </c>
-      <c r="E26" s="2">
-        <v>4.3999999999999995</v>
+      <c r="E26">
+        <v>14.399999999999999</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D27" s="2">
-        <v>146</v>
-      </c>
-      <c r="E27" s="2">
-        <v>40.555555555555557</v>
+        <v>9</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27">
+        <v>77</v>
+      </c>
+      <c r="E27">
+        <v>21.388888888888889</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="2">
-        <v>85</v>
-      </c>
-      <c r="E28" s="2">
-        <v>23.611111111111111</v>
+        <v>9</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>54</v>
+      </c>
+      <c r="E28">
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="2">
-        <v>83</v>
-      </c>
-      <c r="E29" s="2">
-        <v>23.055555555555557</v>
+      <c r="D29">
+        <v>77</v>
+      </c>
+      <c r="E29">
+        <v>21.388888888888889</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="2">
-        <v>23</v>
-      </c>
-      <c r="E30" s="2">
-        <v>6.3888888888888884</v>
+        <v>9</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30">
+        <v>86</v>
+      </c>
+      <c r="E30">
+        <v>23.888888888888889</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>31</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D31" s="2">
-        <v>23</v>
-      </c>
-      <c r="E31" s="2">
-        <v>6.3888888888888884</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="2">
-        <v>104</v>
-      </c>
-      <c r="E32" s="2">
-        <v>37.81818181818182</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="2">
-        <v>80</v>
-      </c>
-      <c r="E33" s="2">
-        <v>29.09090909090909</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>12</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D34" s="2">
-        <v>52</v>
-      </c>
-      <c r="E34" s="2">
-        <v>18.90909090909091</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="2">
-        <v>24</v>
-      </c>
-      <c r="E35" s="2">
-        <v>8.7272727272727284</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>12</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D36" s="2">
-        <v>15</v>
-      </c>
-      <c r="E36" s="2">
-        <v>5.4545454545454541</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>12</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D37" s="2">
-        <v>89</v>
-      </c>
-      <c r="E37" s="2">
-        <v>35.6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="2">
-        <v>77</v>
-      </c>
-      <c r="E38" s="2">
-        <v>30.8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D39" s="2">
-        <v>54</v>
-      </c>
-      <c r="E39" s="2">
-        <v>21.6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" s="2">
-        <v>18</v>
-      </c>
-      <c r="E40" s="2">
-        <v>7.1999999999999993</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>12</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D41" s="2">
-        <v>12</v>
-      </c>
-      <c r="E41" s="2">
-        <v>4.8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>12</v>
-      </c>
-      <c r="B42" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D42" s="2">
-        <v>143</v>
-      </c>
-      <c r="E42" s="2">
-        <v>39.722222222222221</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>12</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43" s="2">
-        <v>86</v>
-      </c>
-      <c r="E43" s="2">
-        <v>23.888888888888889</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D44" s="2">
-        <v>85</v>
-      </c>
-      <c r="E44" s="2">
-        <v>23.611111111111111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>12</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D45" s="2">
-        <v>19</v>
-      </c>
-      <c r="E45" s="2">
-        <v>5.2777777777777777</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="D46" s="2">
-        <v>27</v>
-      </c>
-      <c r="E46" s="2">
-        <v>7.5</v>
+      <c r="D31">
+        <v>66</v>
+      </c>
+      <c r="E31">
+        <v>18.333333333333332</v>
       </c>
     </row>
   </sheetData>
@@ -1644,17 +1387,18 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C18683B-ECE9-E342-B333-4B4395343288}">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B1A2CD-7257-4546-905E-E1227DE5994D}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="50.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1675,123 +1419,513 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>4.7272727272727275</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
+      <c r="E4">
+        <v>11.636363636363637</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="D5">
+        <v>66</v>
+      </c>
+      <c r="E5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6">
+        <v>153</v>
+      </c>
+      <c r="E6">
+        <v>55.63636363636364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+      <c r="E7">
+        <v>4.3999999999999995</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="D9">
+        <v>25</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>64</v>
+      </c>
+      <c r="E10">
+        <v>25.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>137</v>
+      </c>
+      <c r="E11">
+        <v>54.800000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>14.444444444444443</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>76</v>
+      </c>
+      <c r="E15">
+        <v>21.111111111111111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16">
+        <v>192</v>
+      </c>
+      <c r="E16">
+        <v>53.333333333333336</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>1.0909090909090911</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18">
+        <v>11</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+      <c r="E19">
+        <v>7.2727272727272725</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20">
+        <v>55</v>
+      </c>
+      <c r="E20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>186</v>
+      </c>
+      <c r="E21">
+        <v>67.63636363636364</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22">
+        <v>5</v>
+      </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>2.8000000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25">
+        <v>59</v>
+      </c>
+      <c r="E25">
+        <v>23.599999999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="D26">
+        <v>156</v>
+      </c>
+      <c r="E26">
+        <v>62.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>2</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27">
+        <v>7</v>
+      </c>
+      <c r="E27">
+        <v>1.9444444444444444</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>19</v>
+      </c>
+      <c r="E28">
+        <v>5.2777777777777777</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29">
+        <v>39</v>
+      </c>
+      <c r="E29">
+        <v>10.833333333333334</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="11" t="s">
+      <c r="D30">
+        <v>78</v>
+      </c>
+      <c r="E30">
+        <v>21.666666666666668</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>36</v>
+      <c r="D31">
+        <v>217</v>
+      </c>
+      <c r="E31">
+        <v>60.277777777777771</v>
       </c>
     </row>
   </sheetData>
@@ -2298,7 +2432,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A5" sqref="A5:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2430,7 +2564,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2750,20 +2884,21 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE14A6B8-8635-FA4B-AD2A-DEC86D61E5E2}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="B1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="46.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2780,48 +2915,54 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>32</v>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="2">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>54.54545454545454</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.0909090909090911</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>33</v>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D3" s="2">
-        <v>96</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2">
-        <v>34.909090909090914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3.2727272727272729</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="2">
@@ -2830,83 +2971,98 @@
       <c r="E4" s="2">
         <v>6.1818181818181817</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="10"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>35</v>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D5" s="2">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="E5" s="2">
-        <v>3.2727272727272729</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>34.909090909090914</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>36</v>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D6" s="2">
-        <v>3</v>
+        <v>150</v>
       </c>
       <c r="E6" s="2">
-        <v>1.0909090909090911</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54.54545454545454</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>32</v>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D7" s="2">
-        <v>160</v>
+        <v>4</v>
       </c>
       <c r="E7" s="2">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.6</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>33</v>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="2">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="E8" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.6</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="2">
@@ -2915,83 +3071,98 @@
       <c r="E9" s="2">
         <v>6.8000000000000007</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="10"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>35</v>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D10" s="2">
-        <v>4</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>36</v>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D11" s="2">
-        <v>4</v>
+        <v>160</v>
       </c>
       <c r="E11" s="2">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>32</v>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D12" s="2">
-        <v>220</v>
+        <v>7</v>
       </c>
       <c r="E12" s="2">
-        <v>61.111111111111114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.9444444444444444</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>33</v>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="2">
-        <v>88</v>
+        <v>9</v>
       </c>
       <c r="E13" s="2">
-        <v>24.444444444444443</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.5</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="11" t="s">
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D14" s="2">
@@ -3000,83 +3171,98 @@
       <c r="E14" s="2">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="10"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>35</v>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D15" s="2">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="E15" s="2">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24.444444444444443</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>36</v>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D16" s="2">
-        <v>7</v>
+        <v>220</v>
       </c>
       <c r="E16" s="2">
-        <v>1.9444444444444444</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61.111111111111114</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>32</v>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D17" s="2">
-        <v>164</v>
+        <v>6</v>
       </c>
       <c r="E17" s="3">
-        <v>59.636363600000003</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2.1818181800000001</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>33</v>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D18" s="2">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="E18" s="3">
-        <v>19.636363599999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3.2727272699999999</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="11" t="s">
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D19" s="2">
@@ -3085,83 +3271,98 @@
       <c r="E19" s="3">
         <v>15.2727273</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="10"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>35</v>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D20" s="2">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="E20" s="3">
-        <v>3.2727272699999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>19.636363599999999</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>36</v>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D21" s="2">
-        <v>6</v>
+        <v>164</v>
       </c>
       <c r="E21" s="3">
-        <v>2.1818181800000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>59.636363600000003</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>32</v>
+      <c r="C22" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D22" s="2">
-        <v>141</v>
+        <v>4</v>
       </c>
       <c r="E22" s="2">
-        <v>56.399999999999991</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>1.6</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="11" t="s">
-        <v>33</v>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D23" s="2">
-        <v>67</v>
+        <v>5</v>
       </c>
       <c r="E23" s="2">
-        <v>26.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D24" s="2">
@@ -3170,83 +3371,98 @@
       <c r="E24" s="2">
         <v>13.200000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="10"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>35</v>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="2">
-        <v>5</v>
+        <v>67</v>
       </c>
       <c r="E25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+        <v>26.8</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>36</v>
+      <c r="C26" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="2">
-        <v>4</v>
+        <v>141</v>
       </c>
       <c r="E26" s="2">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56.399999999999991</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>32</v>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>36</v>
       </c>
       <c r="D27" s="2">
-        <v>216</v>
+        <v>11</v>
       </c>
       <c r="E27" s="2">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>3.0555555555555554</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>33</v>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
       </c>
       <c r="D28" s="2">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="E28" s="2">
-        <v>21.388888888888889</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>4.1666666666666661</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="11" t="s">
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>34</v>
       </c>
       <c r="D29" s="2">
@@ -3255,40 +3471,49 @@
       <c r="E29" s="2">
         <v>11.388888888888889</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="10"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>35</v>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="D30" s="2">
-        <v>15</v>
+        <v>77</v>
       </c>
       <c r="E30" s="2">
-        <v>4.1666666666666661</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>21.388888888888889</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>36</v>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="2">
-        <v>11</v>
+        <v>216</v>
       </c>
       <c r="E31" s="2">
-        <v>3.0555555555555554</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3296,13 +3521,939 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14B1A2CD-7257-4546-905E-E1227DE5994D}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ABF019-0EA5-9346-A662-004F30A49F1A}">
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="2">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8.7272727272727284</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8.3636363636363633</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="2">
+        <v>70</v>
+      </c>
+      <c r="E4" s="2">
+        <v>25.454545454545453</v>
+      </c>
+      <c r="F4" s="10"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="2">
+        <v>84</v>
+      </c>
+      <c r="E5" s="2">
+        <v>30.545454545454547</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2">
+        <v>74</v>
+      </c>
+      <c r="E6" s="2">
+        <v>26.90909090909091</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="2">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.7999999999999989</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2">
+        <v>17</v>
+      </c>
+      <c r="E8" s="2">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="2">
+        <v>61</v>
+      </c>
+      <c r="E9" s="2">
+        <v>24.4</v>
+      </c>
+      <c r="F9" s="10"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="2">
+        <v>56</v>
+      </c>
+      <c r="E10" s="2">
+        <v>22.400000000000002</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="2">
+        <v>94</v>
+      </c>
+      <c r="E11" s="2">
+        <v>37.6</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="2">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2">
+        <v>11.111111111111111</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="2">
+        <v>22</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6.1111111111111107</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="2">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2">
+        <v>21.388888888888889</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2">
+        <v>67</v>
+      </c>
+      <c r="E15" s="2">
+        <v>18.611111111111111</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2">
+        <v>154</v>
+      </c>
+      <c r="E16" s="2">
+        <v>42.777777777777779</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2">
+        <v>15</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5.4545454545454541</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="2">
+        <v>25</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="2">
+        <v>64</v>
+      </c>
+      <c r="E19" s="2">
+        <v>23.272727272727273</v>
+      </c>
+      <c r="F19" s="10"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="2">
+        <v>95</v>
+      </c>
+      <c r="E20" s="2">
+        <v>34.545454545454547</v>
+      </c>
+      <c r="F20" s="10"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="2">
+        <v>76</v>
+      </c>
+      <c r="E21" s="2">
+        <v>27.636363636363637</v>
+      </c>
+      <c r="F21" s="10"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="2">
+        <v>11</v>
+      </c>
+      <c r="E22" s="2">
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="F22" s="10"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="2">
+        <v>13</v>
+      </c>
+      <c r="E23" s="2">
+        <v>5.2</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2">
+        <v>66</v>
+      </c>
+      <c r="E24" s="2">
+        <v>26.400000000000002</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="2">
+        <v>79</v>
+      </c>
+      <c r="E25" s="2">
+        <v>31.6</v>
+      </c>
+      <c r="F25" s="10"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="2">
+        <v>81</v>
+      </c>
+      <c r="E26" s="2">
+        <v>32.4</v>
+      </c>
+      <c r="F26" s="10"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="2">
+        <v>23</v>
+      </c>
+      <c r="E27" s="2">
+        <v>6.3888888888888884</v>
+      </c>
+      <c r="F27" s="10"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="2">
+        <v>23</v>
+      </c>
+      <c r="E28" s="2">
+        <v>6.3888888888888884</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="2">
+        <v>83</v>
+      </c>
+      <c r="E29" s="2">
+        <v>23.055555555555557</v>
+      </c>
+      <c r="F29" s="10"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" s="2">
+        <v>85</v>
+      </c>
+      <c r="E30" s="2">
+        <v>23.611111111111111</v>
+      </c>
+      <c r="F30" s="10"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="2">
+        <v>146</v>
+      </c>
+      <c r="E31" s="2">
+        <v>40.555555555555557</v>
+      </c>
+      <c r="F31" s="10"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D32" s="2">
+        <v>15</v>
+      </c>
+      <c r="E32" s="2">
+        <v>5.4545454545454541</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D33" s="2">
+        <v>24</v>
+      </c>
+      <c r="E33" s="2">
+        <v>8.7272727272727284</v>
+      </c>
+      <c r="F33" s="10"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="2">
+        <v>52</v>
+      </c>
+      <c r="E34" s="2">
+        <v>18.90909090909091</v>
+      </c>
+      <c r="F34" s="10"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="2">
+        <v>80</v>
+      </c>
+      <c r="E35" s="2">
+        <v>29.09090909090909</v>
+      </c>
+      <c r="F35" s="10"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="2">
+        <v>104</v>
+      </c>
+      <c r="E36" s="2">
+        <v>37.81818181818182</v>
+      </c>
+      <c r="F36" s="10"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="2">
+        <v>12</v>
+      </c>
+      <c r="E37" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F37" s="10"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D38" s="2">
+        <v>18</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D39" s="2">
+        <v>54</v>
+      </c>
+      <c r="E39" s="2">
+        <v>21.6</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="2">
+        <v>77</v>
+      </c>
+      <c r="E40" s="2">
+        <v>30.8</v>
+      </c>
+      <c r="F40" s="10"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D41" s="2">
+        <v>89</v>
+      </c>
+      <c r="E41" s="2">
+        <v>35.6</v>
+      </c>
+      <c r="F41" s="10"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="2">
+        <v>27</v>
+      </c>
+      <c r="E42" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="F42" s="10"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="2">
+        <v>19</v>
+      </c>
+      <c r="E43" s="2">
+        <v>5.2777777777777777</v>
+      </c>
+      <c r="F43" s="10"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D44" s="2">
+        <v>85</v>
+      </c>
+      <c r="E44" s="2">
+        <v>23.611111111111111</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="2">
+        <v>86</v>
+      </c>
+      <c r="E45" s="2">
+        <v>23.888888888888889</v>
+      </c>
+      <c r="F45" s="10"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D46" s="2">
+        <v>143</v>
+      </c>
+      <c r="E46" s="2">
+        <v>39.722222222222221</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>